<commit_message>
add temp-timout parameter to excel config file. fix to read the pressure befor write the calib point to DP
</commit_message>
<xml_diff>
--- a/test1_config.xlsx
+++ b/test1_config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>pressure[bar]</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Delta[c]</t>
+  </si>
+  <si>
+    <t>Temp timout[Min]</t>
   </si>
 </sst>
 </file>
@@ -272,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -341,6 +344,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -644,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,13 +668,15 @@
     <col min="2" max="2" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="8.88671875" style="1"/>
     <col min="7" max="7" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.88671875" style="1"/>
-    <col min="10" max="10" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="1"/>
+    <col min="11" max="11" width="36" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
@@ -670,7 +684,7 @@
       <c r="C1" s="16"/>
       <c r="D1" s="17"/>
     </row>
-    <row r="2" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -685,8 +699,9 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="21"/>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
@@ -701,8 +716,9 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -711,183 +727,207 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L5" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="I6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="14"/>
-    </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L6" s="14"/>
+    </row>
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G7" s="4">
         <v>0</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="24">
         <v>25.6</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="I7" s="5">
+        <v>20</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="L7" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G8" s="4">
         <v>0.34</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="24">
         <v>28</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="I8" s="5"/>
+      <c r="K8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G9" s="4">
         <v>0.7</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="J9" s="12" t="s">
+      <c r="H9" s="24"/>
+      <c r="I9" s="5"/>
+      <c r="K9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L9" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G10" s="4">
         <v>1</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="J10" s="12" t="s">
+      <c r="H10" s="24"/>
+      <c r="I10" s="5"/>
+      <c r="K10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L10" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G11" s="4">
         <v>1.4</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="J11" s="12" t="s">
+      <c r="H11" s="24"/>
+      <c r="I11" s="5"/>
+      <c r="K11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="5">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L11" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G12" s="4">
         <v>1.75</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="J12" s="12" t="s">
+      <c r="H12" s="24"/>
+      <c r="I12" s="5"/>
+      <c r="K12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="5">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L12" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G13" s="4">
         <v>2.1</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="5"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H13" s="24"/>
+      <c r="I13" s="5"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G14" s="4">
         <v>2.4500000000000002</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H14" s="24"/>
+      <c r="I14" s="5"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G15" s="4">
         <v>2.8</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H15" s="24"/>
+      <c r="I15" s="5"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="G16" s="4">
         <v>3.5</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="H16" s="24"/>
+      <c r="I16" s="5"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G17" s="4">
         <v>4.3</v>
       </c>
-      <c r="H17" s="5"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="H17" s="24"/>
+      <c r="I17" s="5"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G18" s="4">
         <v>5.05</v>
       </c>
-      <c r="H18" s="5"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H18" s="24"/>
+      <c r="I18" s="5"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="7:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G19" s="4">
         <v>5.8</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="7"/>
-    </row>
-    <row r="20" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="H19" s="24"/>
+      <c r="I19" s="5"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G20" s="4">
         <v>6.55</v>
       </c>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="H20" s="24"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G21" s="4">
         <v>6.7</v>
       </c>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="H21" s="24"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G22" s="4"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="H22" s="24"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="7:12" x14ac:dyDescent="0.3">
       <c r="G23" s="4"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="7:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H23" s="24"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="7:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G24" s="6"/>
-      <c r="H24" s="7"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="K6:L6"/>
     <mergeCell ref="A1:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>